<commit_message>
perdon q insista con el EXCEL
</commit_message>
<xml_diff>
--- a/EXCEL.xlsx
+++ b/EXCEL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="23715" windowHeight="10050" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="20640" windowHeight="10050" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -138,6 +138,41 @@
     <author>Eugenio Arevalo</author>
   </authors>
   <commentList>
+    <comment ref="J2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eugenio Arevalo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+codigo de Cliente en entidad
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eugenio Arevalo</author>
+  </authors>
+  <commentList>
     <comment ref="G10" authorId="0">
       <text>
         <r>
@@ -167,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="274">
   <si>
     <t>fila[]</t>
   </si>
@@ -787,9 +822,6 @@
     <t>CONTABLE</t>
   </si>
   <si>
-    <t>ARCHIVO FACTURAS</t>
-  </si>
-  <si>
     <t>IMPUTACION</t>
   </si>
   <si>
@@ -947,13 +979,58 @@
   </si>
   <si>
     <t>Metodos de clase</t>
+  </si>
+  <si>
+    <t>CTA</t>
+  </si>
+  <si>
+    <t>COMPRA</t>
+  </si>
+  <si>
+    <t>SALDO</t>
+  </si>
+  <si>
+    <t>DUPLICADO</t>
+  </si>
+  <si>
+    <t>COD ENTI</t>
+  </si>
+  <si>
+    <t>TIPO ENT</t>
+  </si>
+  <si>
+    <t>VINO TITO</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>Venta Vet[Cant++]</t>
+  </si>
+  <si>
+    <t>detalle_vta</t>
+  </si>
+  <si>
+    <t>subTotalProd</t>
+  </si>
+  <si>
+    <t>A TotalProd</t>
+  </si>
+  <si>
+    <t>planCta</t>
+  </si>
+  <si>
+    <t>codEnt</t>
+  </si>
+  <si>
+    <t>DETALLE FACTURA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1071,6 +1148,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -1165,7 +1250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1261,6 +1346,19 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1281,6 +1379,18 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2213,97 +2323,683 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="1"/>
+    <col min="9" max="9" width="11.42578125" style="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="55" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" s="13" t="s">
+      <c r="F2" s="51" t="s">
         <v>224</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="I2" s="51" t="s">
+        <v>261</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="M2" s="23">
+        <v>100</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="36">
         <v>43789</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="16">
+        <v>1</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="16">
+      <c r="F3" s="53">
+        <v>4132.2299999999996</v>
+      </c>
+      <c r="G3" s="53"/>
+      <c r="H3" s="15">
+        <v>105</v>
+      </c>
+      <c r="I3" s="53">
+        <f>+F3-G3</f>
+        <v>4132.2299999999996</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="K3" s="15">
+        <v>1153</v>
+      </c>
+      <c r="M3" s="20">
+        <v>101</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="36">
+        <v>43789</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="16">
         <v>1</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="E4" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53">
+        <v>5000</v>
+      </c>
+      <c r="H4" s="15">
+        <v>102</v>
+      </c>
+      <c r="I4" s="53">
+        <f t="shared" ref="I4:I15" si="0">+F4-G4</f>
+        <v>-5000</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="K4" s="15">
+        <v>1153</v>
+      </c>
+      <c r="M4" s="22">
+        <v>102</v>
+      </c>
+      <c r="N4" s="22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="36">
+        <v>43789</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="16">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="F5" s="53">
+        <v>867.77</v>
+      </c>
+      <c r="G5" s="53"/>
+      <c r="H5" s="15">
+        <v>204</v>
+      </c>
+      <c r="I5" s="53">
+        <f t="shared" si="0"/>
+        <v>867.77</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="K5" s="15">
+        <v>1153</v>
+      </c>
+      <c r="M5" s="22">
+        <v>103</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="36">
+        <v>43790</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="16">
+        <v>4</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53">
+        <v>85.71</v>
+      </c>
+      <c r="H6" s="15"/>
+      <c r="I6" s="53">
+        <f t="shared" si="0"/>
+        <v>-85.71</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="15">
+        <v>1154</v>
+      </c>
+      <c r="M6" s="22">
+        <v>104</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="36">
+        <v>43790</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="16">
+        <v>4</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="F7" s="53">
+        <v>120</v>
+      </c>
+      <c r="G7" s="53"/>
+      <c r="H7" s="15">
+        <v>102</v>
+      </c>
+      <c r="I7" s="53">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="15">
+        <v>1154</v>
+      </c>
+      <c r="M7" s="20">
+        <v>105</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="36">
+        <v>43790</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="16">
+        <v>4</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53">
+        <v>34.29</v>
+      </c>
+      <c r="H8" s="15">
+        <v>203</v>
+      </c>
+      <c r="I8" s="53">
+        <f t="shared" si="0"/>
+        <v>-34.29</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="15">
+        <v>1154</v>
+      </c>
+      <c r="M8" s="20">
+        <v>106</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="M9" s="20">
+        <v>107</v>
+      </c>
+      <c r="N9" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="M10" s="20">
+        <v>108</v>
+      </c>
+      <c r="N10" s="20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="M11" s="23">
+        <v>200</v>
+      </c>
+      <c r="N11" s="23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="M12" s="20">
+        <v>201</v>
+      </c>
+      <c r="N12" s="20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="M13" s="22">
+        <v>202</v>
+      </c>
+      <c r="N13" s="22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="M14" s="22">
+        <v>203</v>
+      </c>
+      <c r="N14" s="22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F15" s="52">
+        <f>SUM(F3:F14)</f>
+        <v>5120</v>
+      </c>
+      <c r="G15" s="52">
+        <f>SUM(G3:G14)</f>
+        <v>5120</v>
+      </c>
+      <c r="H15" s="50"/>
+      <c r="I15" s="52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="22">
+        <v>204</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M16" s="22">
+        <v>205</v>
+      </c>
+      <c r="N16" s="22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M17" s="22">
+        <v>206</v>
+      </c>
+      <c r="N17" s="22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M18" s="20">
+        <v>208</v>
+      </c>
+      <c r="N18" s="20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M19" s="20">
+        <v>209</v>
+      </c>
+      <c r="N19" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M20" s="20">
+        <v>210</v>
+      </c>
+      <c r="N20" s="21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M21" s="23">
+        <v>300</v>
+      </c>
+      <c r="N21" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M22" s="20">
+        <v>301</v>
+      </c>
+      <c r="N22" s="21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M23" s="20">
+        <v>302</v>
+      </c>
+      <c r="N23" s="20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M24" s="20">
+        <v>303</v>
+      </c>
+      <c r="N24" s="21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M25" s="20">
+        <v>304</v>
+      </c>
+      <c r="N25" s="20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M26" s="20">
+        <v>305</v>
+      </c>
+      <c r="N26" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M27" s="23">
+        <v>400</v>
+      </c>
+      <c r="N27" s="23" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M28" s="22">
+        <v>401</v>
+      </c>
+      <c r="N28" s="22" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M29" s="20">
+        <v>402</v>
+      </c>
+      <c r="N29" s="20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M30" s="20">
+        <v>403</v>
+      </c>
+      <c r="N30" s="20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M31" s="23">
+        <v>500</v>
+      </c>
+      <c r="N31" s="23" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="32" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M32" s="22">
+        <v>501</v>
+      </c>
+      <c r="N32" s="22" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M33" s="20">
+        <v>502</v>
+      </c>
+      <c r="N33" s="20" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M34" s="22">
+        <v>503</v>
+      </c>
+      <c r="N34" s="22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="35" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M35" s="22">
+        <v>506</v>
+      </c>
+      <c r="N35" s="22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M36" s="22">
+        <v>507</v>
+      </c>
+      <c r="N36" s="22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="37" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M37" s="20">
+        <v>508</v>
+      </c>
+      <c r="N37" s="20" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M38" s="22">
+        <v>509</v>
+      </c>
+      <c r="N38" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M39" s="22">
+        <v>513</v>
+      </c>
+      <c r="N39" s="22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M40" s="20">
+        <v>515</v>
+      </c>
+      <c r="N40" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="13:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M41" s="20">
+        <v>516</v>
+      </c>
+      <c r="N41" s="20" t="s">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2312,7 +3008,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2329,33 +3025,33 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="54" t="s">
         <v>258</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="55" t="s">
+      <c r="C1" s="59" t="s">
         <v>257</v>
       </c>
-      <c r="F1" s="55"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="60" t="s">
+        <v>256</v>
+      </c>
+      <c r="F1" s="60"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2363,44 +3059,44 @@
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="40" t="s">
+        <v>241</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F9" s="46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" s="45" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F10" s="40">
         <v>9</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G11" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H11" s="42">
         <v>700</v>
@@ -2416,18 +3112,18 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G13" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H13" s="46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I14" s="43" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J14" s="42">
         <v>1400</v>
@@ -2435,26 +3131,26 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="42" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>208</v>
+        <v>268</v>
       </c>
       <c r="I16" s="46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D17" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K17" s="42">
         <f>+J14</f>
@@ -2463,10 +3159,10 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C18" s="46" t="s">
-        <v>208</v>
+        <v>268</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K18" s="42">
         <f>+K17*0.95</f>
@@ -2475,10 +3171,10 @@
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D19" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K19" s="42">
         <f>+K18*21/100</f>
@@ -2487,10 +3183,10 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D20" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K20" s="42">
         <f>+K18+K19</f>
@@ -2499,17 +3195,17 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D21" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="42" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -2542,7 +3238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -2575,14 +3271,14 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="54" t="s">
         <v>174</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F3" s="25"/>
@@ -2992,28 +3688,29 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -3029,13 +3726,13 @@
         <v>125</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F2" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>228</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>229</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>126</v>
@@ -3345,25 +4042,25 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
-        <v>239</v>
-      </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
+      <c r="A13" s="56" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="52">
+      <c r="A14" s="57">
         <v>40</v>
       </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G15" s="37"/>
     </row>
     <row r="20" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3382,7 +4079,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3399,17 +4096,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -3725,8 +4422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3743,17 +4440,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -3962,7 +4659,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection sqref="A1:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3973,10 +4670,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>214</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4003,10 +4700,10 @@
         <v>138</v>
       </c>
       <c r="C4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" t="s">
         <v>240</v>
-      </c>
-      <c r="D4" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4190,7 +4887,7 @@
         <v>400</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4201,7 +4898,7 @@
         <v>159</v>
       </c>
       <c r="D28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4209,7 +4906,7 @@
         <v>402</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4225,7 +4922,7 @@
         <v>500</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4236,7 +4933,7 @@
         <v>161</v>
       </c>
       <c r="C32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -4320,423 +5017,478 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
-        <v>206</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>193</v>
-      </c>
       <c r="G2" s="11" t="s">
-        <v>194</v>
+        <v>269</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="I2" s="32" t="s">
-        <v>198</v>
+        <v>270</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>271</v>
       </c>
       <c r="J2" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="L2" s="32" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="29">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="49">
+        <v>1</v>
+      </c>
+      <c r="B3" s="29">
         <v>100</v>
       </c>
-      <c r="B3" s="30">
+      <c r="C3" s="30">
         <v>2</v>
       </c>
-      <c r="C3" s="30">
+      <c r="D3" s="30">
         <v>6</v>
       </c>
-      <c r="D3" s="29">
+      <c r="E3" s="62">
         <v>110</v>
       </c>
-      <c r="E3" s="29">
+      <c r="F3" s="62">
         <v>138.6</v>
       </c>
-      <c r="F3" s="29">
+      <c r="G3" s="62">
         <v>660</v>
       </c>
-      <c r="G3" s="31">
-        <f>+E3+F3</f>
+      <c r="H3" s="63">
+        <f>+F3+G3</f>
         <v>798.6</v>
       </c>
-      <c r="H3" s="29">
+      <c r="I3" s="29">
         <v>102</v>
       </c>
-      <c r="I3" s="33">
+      <c r="J3" s="33">
         <v>5</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="K3" s="33">
+        <v>1</v>
+      </c>
+      <c r="L3" s="33" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="29">
+      <c r="S3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="49">
+        <v>2</v>
+      </c>
+      <c r="B4" s="29">
         <v>100</v>
       </c>
-      <c r="B4" s="30">
+      <c r="C4" s="30">
         <v>3</v>
       </c>
-      <c r="C4" s="30">
+      <c r="D4" s="30">
         <v>6</v>
       </c>
-      <c r="D4" s="29">
+      <c r="E4" s="62">
         <v>210</v>
       </c>
-      <c r="E4" s="29">
+      <c r="F4" s="62">
         <v>264.60000000000002</v>
       </c>
-      <c r="F4" s="29">
+      <c r="G4" s="62">
         <v>1260</v>
       </c>
-      <c r="G4" s="31">
-        <f>+E4+F4</f>
+      <c r="H4" s="63">
+        <f>+F4+G4</f>
         <v>1524.6</v>
       </c>
-      <c r="H4" s="29">
+      <c r="I4" s="29">
         <v>102</v>
       </c>
-      <c r="I4" s="33">
+      <c r="J4" s="33">
         <v>5</v>
       </c>
-      <c r="J4" s="33" t="s">
+      <c r="K4" s="33">
+        <v>1</v>
+      </c>
+      <c r="L4" s="33" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="49">
+        <v>3</v>
+      </c>
+      <c r="B5" s="29">
+        <v>101</v>
+      </c>
+      <c r="C5" s="30">
+        <v>2</v>
+      </c>
+      <c r="D5" s="30">
+        <v>1</v>
+      </c>
+      <c r="E5" s="62">
+        <v>110</v>
+      </c>
+      <c r="F5" s="62">
+        <v>23.21</v>
+      </c>
+      <c r="G5" s="62">
+        <v>110</v>
+      </c>
+      <c r="H5" s="64">
+        <v>133.21</v>
+      </c>
+      <c r="I5" s="29">
+        <v>102</v>
+      </c>
+      <c r="J5" s="33">
+        <v>16</v>
+      </c>
+      <c r="K5" s="33">
+        <v>1</v>
+      </c>
+      <c r="L5" s="33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="16"/>
-      <c r="D6" s="15"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="17"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="15"/>
       <c r="J6" s="17"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="16"/>
-      <c r="D7" s="15"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="17"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="15"/>
       <c r="J7" s="17"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="25"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="25"/>
+      <c r="G14" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="H14" s="25" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="25"/>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
       <c r="F15" s="25"/>
       <c r="G15" s="25"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="25" t="s">
+      <c r="H15" s="25"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C16" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="E16" s="25"/>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="25"/>
+      <c r="G16" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="G16" s="25"/>
-      <c r="J16">
+      <c r="H16" s="25"/>
+      <c r="L16">
         <v>1000</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <v>0.21</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C17" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="C17" s="25"/>
       <c r="D17" s="25"/>
       <c r="E17" s="25"/>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="25"/>
+      <c r="G17" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="G17" s="25"/>
-      <c r="K17">
-        <f>+J16*K16</f>
+      <c r="H17" s="25"/>
+      <c r="M17">
+        <f>+L16*M16</f>
         <v>210</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="25" t="s">
+    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C18" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="C18" s="25"/>
       <c r="D18" s="25"/>
       <c r="E18" s="25"/>
-      <c r="F18" s="25" t="s">
+      <c r="F18" s="25"/>
+      <c r="G18" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="G18" s="25"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="25" t="s">
+      <c r="H18" s="25"/>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C19" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="C19" s="25"/>
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="25"/>
+      <c r="G19" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="G19" s="25"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="25" t="s">
+      <c r="H19" s="25"/>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C20" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="C20" s="25"/>
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="25"/>
+      <c r="G20" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="G20" s="25"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="25"/>
+      <c r="H20" s="25"/>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
       <c r="G21" s="25"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="24" t="s">
+      <c r="H21" s="25"/>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C22" s="61" t="s">
         <v>181</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="D22" s="61" t="s">
         <v>182</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="E22" s="61" t="s">
         <v>183</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="F22" s="61" t="s">
         <v>184</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="G22" s="61" t="s">
         <v>189</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="H22" s="61" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="25">
+    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C23" s="25">
         <v>2</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="D23" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D23" s="25">
+      <c r="E23" s="25">
         <v>6</v>
       </c>
-      <c r="E23" s="25">
+      <c r="F23" s="25">
         <v>110</v>
       </c>
-      <c r="F23" s="25">
-        <f>+G23*21/100</f>
+      <c r="G23" s="25">
+        <f>+H23*21/100</f>
         <v>138.6</v>
       </c>
-      <c r="G23" s="25">
-        <f>+E23*D23</f>
+      <c r="H23" s="25">
+        <f>+F23*E23</f>
         <v>660</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="25">
+    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C24" s="25">
         <v>3</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="D24" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="D24" s="25">
+      <c r="E24" s="25">
         <v>6</v>
       </c>
-      <c r="E24" s="25">
+      <c r="F24" s="25">
         <v>210</v>
       </c>
-      <c r="F24" s="25">
-        <f>+G24*21/100</f>
+      <c r="G24" s="25">
+        <f>+H24*21/100</f>
         <v>264.60000000000002</v>
       </c>
-      <c r="G24" s="25">
-        <f>+E24*D24</f>
+      <c r="H24" s="25">
+        <f>+F24*E24</f>
         <v>1260</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="25"/>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C25" s="25"/>
       <c r="D25" s="25"/>
       <c r="E25" s="25"/>
       <c r="F25" s="25"/>
       <c r="G25" s="25"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="25"/>
+      <c r="H25" s="25"/>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C26" s="25"/>
       <c r="D26" s="25"/>
       <c r="E26" s="25"/>
       <c r="F26" s="25"/>
       <c r="G26" s="25"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="25"/>
+      <c r="H26" s="25"/>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C27" s="25"/>
       <c r="D27" s="25"/>
       <c r="E27" s="25"/>
       <c r="F27" s="25"/>
       <c r="G27" s="25"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="25"/>
+      <c r="H27" s="25"/>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C28" s="25"/>
       <c r="D28" s="25"/>
       <c r="E28" s="25"/>
       <c r="F28" s="25"/>
       <c r="G28" s="25"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="25"/>
+      <c r="H28" s="25"/>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C29" s="25"/>
       <c r="D29" s="25"/>
       <c r="E29" s="25"/>
       <c r="F29" s="25"/>
       <c r="G29" s="25"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="26"/>
+      <c r="H29" s="25"/>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
       <c r="E30" s="26"/>
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="26"/>
+      <c r="G30" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="G30" s="27">
-        <f>SUM(G23:G29)</f>
+      <c r="H30" s="27">
+        <f>SUM(H23:H29)</f>
         <v>1920</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="26"/>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
       <c r="E31" s="26"/>
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="26"/>
+      <c r="G31" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="G31" s="27">
-        <f>+F23+F24</f>
+      <c r="H31" s="27">
+        <f>+G23+G24</f>
         <v>403.20000000000005</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="26"/>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
       <c r="E32" s="26"/>
-      <c r="F32" s="26" t="s">
+      <c r="F32" s="26"/>
+      <c r="G32" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="G32" s="27">
-        <f>+G30+G31</f>
+      <c r="H32" s="27">
+        <f>+H30+H31</f>
         <v>2323.1999999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1"/>
-    <hyperlink ref="F17" r:id="rId2"/>
+    <hyperlink ref="C17" r:id="rId1"/>
+    <hyperlink ref="G17" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4744,8 +5496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4754,27 +5506,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="58" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>200</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>203</v>

</xml_diff>